<commit_message>
First commit after publication
</commit_message>
<xml_diff>
--- a/Rawdata to Figure 5_NEW.xlsx
+++ b/Rawdata to Figure 5_NEW.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7620"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sleep during work period AW QW" sheetId="1" r:id="rId1"/>
@@ -84,11 +84,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2272,11 +2274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="626345384"/>
-        <c:axId val="626345776"/>
+        <c:axId val="702037448"/>
+        <c:axId val="702037840"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="626345384"/>
+        <c:axId val="702037448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2286,7 +2288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626345776"/>
+        <c:crossAx val="702037840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2294,7 +2296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="626345776"/>
+        <c:axId val="702037840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2304,7 +2306,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626345384"/>
+        <c:crossAx val="702037448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4660,11 +4662,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="626987224"/>
-        <c:axId val="626987616"/>
+        <c:axId val="754196320"/>
+        <c:axId val="754194752"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="626987224"/>
+        <c:axId val="754196320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4674,7 +4676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626987616"/>
+        <c:crossAx val="754194752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4682,7 +4684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="626987616"/>
+        <c:axId val="754194752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4692,7 +4694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626987224"/>
+        <c:crossAx val="754196320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5999,11 +6001,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="626988400"/>
-        <c:axId val="626988792"/>
+        <c:axId val="784740776"/>
+        <c:axId val="784741168"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="626988400"/>
+        <c:axId val="784740776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6046,7 +6048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="626988792"/>
+        <c:crossAx val="784741168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6056,7 +6058,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="626988792"/>
+        <c:axId val="784741168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6163,7 +6165,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="626988400"/>
+        <c:crossAx val="784740776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7671,11 +7673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="626989576"/>
-        <c:axId val="626989968"/>
+        <c:axId val="784741952"/>
+        <c:axId val="784742344"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="626989576"/>
+        <c:axId val="784741952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7718,7 +7720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="626989968"/>
+        <c:crossAx val="784742344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7726,7 +7728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="626989968"/>
+        <c:axId val="784742344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7841,7 +7843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="626989576"/>
+        <c:crossAx val="784741952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9442,13 +9444,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="BP19" sqref="BP19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -9472,6 +9475,8 @@
     <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" x14ac:dyDescent="0.25">

</xml_diff>